<commit_message>
Sequences with methods for Grouping, Sekecting, searching based on conditions (Where) and getting first element (element) added to the project.
Information in the Excel files to deal with the new methods added.
</commit_message>
<xml_diff>
--- a/Files/Testing LinQ.xlsx
+++ b/Files/Testing LinQ.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Updated Products" sheetId="2" r:id="rId1"/>
     <sheet name="Updated with condition" sheetId="3" r:id="rId2"/>
     <sheet name="Store Items" sheetId="1" r:id="rId3"/>
+    <sheet name="Grouping Info" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="12">
   <si>
     <t>Item</t>
   </si>
@@ -95,9 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +503,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -599,7 +603,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +614,7 @@
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -638,7 +642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -652,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -666,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -680,7 +684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -693,6 +697,23 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
     </row>
     <row r="31" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
@@ -701,4 +722,173 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1500</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>900</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1500</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>900</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>500</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sum and group table values sequence created
</commit_message>
<xml_diff>
--- a/Files/Testing LinQ.xlsx
+++ b/Files/Testing LinQ.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
   <si>
     <t>Item</t>
   </si>
@@ -726,166 +726,100 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
         <v>1500</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
         <v>150</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
         <v>900</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
         <v>30</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
         <v>500</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
         <v>1500</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>15</v>
-      </c>
-      <c r="C8">
         <v>150</v>
       </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>32</v>
-      </c>
-      <c r="C9">
         <v>900</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>12</v>
-      </c>
-      <c r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
         <v>500</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New LinQ methods created for: Ordering, Joining, and getting total sum, average, min as well as their respective tables on Excel
</commit_message>
<xml_diff>
--- a/Files/Testing LinQ.xlsx
+++ b/Files/Testing LinQ.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Updated Products" sheetId="2" r:id="rId1"/>
     <sheet name="Updated with condition" sheetId="3" r:id="rId2"/>
-    <sheet name="Store Items" sheetId="1" r:id="rId3"/>
-    <sheet name="Grouping Info" sheetId="4" r:id="rId4"/>
+    <sheet name="Average" sheetId="5" r:id="rId3"/>
+    <sheet name="Store Items" sheetId="1" r:id="rId4"/>
+    <sheet name="Joins" sheetId="6" r:id="rId5"/>
+    <sheet name="Grouping Info" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="21">
   <si>
     <t>Item</t>
   </si>
@@ -53,13 +55,40 @@
   </si>
   <si>
     <t>Spinning Bycicle</t>
+  </si>
+  <si>
+    <t>Pets</t>
+  </si>
+  <si>
+    <t>Dog Bed</t>
+  </si>
+  <si>
+    <t>Dry food</t>
+  </si>
+  <si>
+    <t>SectionID</t>
+  </si>
+  <si>
+    <t>Grocery</t>
+  </si>
+  <si>
+    <t>Dr Pepper</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Digital Camera</t>
+  </si>
+  <si>
+    <t>JOINED Tables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +104,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,15 +134,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,10 +646,77 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>212.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +727,7 @@
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -642,7 +755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -656,7 +769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -670,7 +783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -678,13 +791,13 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -698,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -706,14 +819,28 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>150</v>
+        <v>275</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
     </row>
     <row r="31" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
@@ -724,11 +851,444 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1500</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>900</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>130</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>275</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>1200</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>1500</v>
+      </c>
+      <c r="O14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>6</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>150</v>
+      </c>
+      <c r="O15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>900</v>
+      </c>
+      <c r="O16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17">
+        <v>10</v>
+      </c>
+      <c r="N17">
+        <v>15</v>
+      </c>
+      <c r="O17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18">
+        <v>20</v>
+      </c>
+      <c r="N18">
+        <v>130</v>
+      </c>
+      <c r="O18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>500</v>
+      </c>
+      <c r="O19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>275</v>
+      </c>
+      <c r="O20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21">
+        <v>100</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <v>30</v>
+      </c>
+      <c r="O22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>14</v>
+      </c>
+      <c r="M23">
+        <v>60</v>
+      </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24">
+        <v>20</v>
+      </c>
+      <c r="N24">
+        <v>5</v>
+      </c>
+      <c r="O24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="12:15" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>1200</v>
+      </c>
+      <c r="O25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N11:P11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>